<commit_message>
Pushing Up Weird Files
</commit_message>
<xml_diff>
--- a/Health/PreHealthConcerns_YouthProgram2.xlsx
+++ b/Health/PreHealthConcerns_YouthProgram2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\FHP\Quant Survey Analysis\GitHubFHP_Repository\Health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57AA211-7A3E-40C5-A1B6-BE8B99344A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C360301-7A9A-4933-9590-2C23743560BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16320" xr2:uid="{16C691A2-71DF-4D9B-A5FF-890B03C32E3E}"/>
+    <workbookView xWindow="5580" yWindow="525" windowWidth="22530" windowHeight="16995" xr2:uid="{16C691A2-71DF-4D9B-A5FF-890B03C32E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,13 +56,13 @@
     <t>Physical (N=28)</t>
   </si>
   <si>
-    <t>Mental (N=43)</t>
-  </si>
-  <si>
     <t>Substance Use (N=6)</t>
   </si>
   <si>
     <t>N=70</t>
+  </si>
+  <si>
+    <t>Mental (N=44)</t>
   </si>
 </sst>
 </file>
@@ -438,17 +438,20 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -501,7 +504,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>44</v>
@@ -515,7 +518,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>6</v>

</xml_diff>